<commit_message>
Update cell cell communication.xlsx
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1365" windowWidth="12855" windowHeight="120"/>
+    <workbookView xWindow="-105" yWindow="1815" windowWidth="12855" windowHeight="120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7672" uniqueCount="7577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7672" uniqueCount="7575">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22658,14 +22658,6 @@
   </si>
   <si>
     <t>pSB1C3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>pSB6A1,pSB1C3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>pSB3K3,pSB1C3</t>
     <phoneticPr fontId="20"/>
   </si>
   <si>
@@ -23606,7 +23598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="L18" sqref="L18:L29"/>
     </sheetView>
   </sheetViews>
@@ -24023,7 +24015,7 @@
     </row>
     <row r="18" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>7570</v>
+        <v>7568</v>
       </c>
       <c r="B18" s="24"/>
       <c r="D18" s="22"/>
@@ -24031,7 +24023,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>7570</v>
+        <v>7568</v>
       </c>
       <c r="J18" s="19" t="b">
         <v>0</v>
@@ -24045,14 +24037,14 @@
     </row>
     <row r="19" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>7571</v>
+        <v>7569</v>
       </c>
       <c r="B19" s="24"/>
       <c r="F19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>7571</v>
+        <v>7569</v>
       </c>
       <c r="J19" s="19" t="b">
         <v>0</v>
@@ -24067,7 +24059,7 @@
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="43" t="s">
-        <v>7572</v>
+        <v>7570</v>
       </c>
       <c r="B20" s="39"/>
       <c r="D20" s="22"/>
@@ -24076,7 +24068,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>7572</v>
+        <v>7570</v>
       </c>
       <c r="J20" s="19" t="b">
         <v>0</v>
@@ -24090,7 +24082,7 @@
     </row>
     <row r="21" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>7573</v>
+        <v>7571</v>
       </c>
       <c r="B21" s="39"/>
       <c r="D21" s="22"/>
@@ -24099,7 +24091,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>7573</v>
+        <v>7571</v>
       </c>
       <c r="J21" s="19" t="b">
         <v>0</v>
@@ -24113,7 +24105,7 @@
     </row>
     <row r="22" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>7574</v>
+        <v>7572</v>
       </c>
       <c r="B22" s="39"/>
       <c r="C22" s="24"/>
@@ -24121,7 +24113,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>7574</v>
+        <v>7572</v>
       </c>
       <c r="J22" s="19" t="b">
         <v>0</v>
@@ -24135,14 +24127,14 @@
     </row>
     <row r="23" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>7567</v>
+        <v>7565</v>
       </c>
       <c r="B23" s="39"/>
       <c r="F23" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>7567</v>
+        <v>7565</v>
       </c>
       <c r="J23" s="19" t="b">
         <v>0</v>
@@ -24178,7 +24170,7 @@
     </row>
     <row r="25" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>7565</v>
+        <v>7563</v>
       </c>
       <c r="B25" s="39"/>
       <c r="D25" s="22"/>
@@ -24186,7 +24178,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>7565</v>
+        <v>7563</v>
       </c>
       <c r="J25" s="19" t="b">
         <v>0</v>
@@ -24200,14 +24192,14 @@
     </row>
     <row r="26" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>7547</v>
+        <v>7545</v>
       </c>
       <c r="B26" s="39"/>
       <c r="F26" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>7547</v>
+        <v>7545</v>
       </c>
       <c r="J26" s="19" t="b">
         <v>0</v>
@@ -24221,7 +24213,7 @@
     </row>
     <row r="27" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>7575</v>
+        <v>7573</v>
       </c>
       <c r="B27" s="39"/>
       <c r="D27" s="22"/>
@@ -24229,7 +24221,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>7575</v>
+        <v>7573</v>
       </c>
       <c r="J27" s="19" t="b">
         <v>0</v>
@@ -24265,7 +24257,7 @@
     </row>
     <row r="29" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>7576</v>
+        <v>7574</v>
       </c>
       <c r="B29" s="39"/>
       <c r="D29" s="22"/>
@@ -24273,7 +24265,7 @@
         <v>8</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>7576</v>
+        <v>7574</v>
       </c>
       <c r="J29" s="19" t="b">
         <v>0</v>
@@ -25299,8 +25291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:K22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -25809,7 +25801,7 @@
         <v>7530</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>7555</v>
+        <v>7553</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>7527</v>
@@ -25818,17 +25810,17 @@
         <v>1</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="43" t="s">
-        <v>7547</v>
+        <v>7545</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>7523</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>7548</v>
+        <v>7546</v>
       </c>
       <c r="J14" s="36"/>
       <c r="K14" s="22"/>
@@ -25853,7 +25845,7 @@
         <v>7531</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>7555</v>
+        <v>7553</v>
       </c>
       <c r="C15" s="44" t="s">
         <v>7528</v>
@@ -25862,19 +25854,19 @@
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="H15" s="42" t="s">
         <v>7523</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>7550</v>
+        <v>7548</v>
       </c>
       <c r="J15" s="42" t="s">
-        <v>7551</v>
+        <v>7549</v>
       </c>
       <c r="K15" s="22"/>
     </row>
@@ -25883,7 +25875,7 @@
         <v>7532</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>7555</v>
+        <v>7553</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>7533</v>
@@ -25892,20 +25884,20 @@
         <v>1</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>7537</v>
+        <v>7536</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="24" t="s">
-        <v>7552</v>
+        <v>7550</v>
       </c>
       <c r="H16" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>7551</v>
+      </c>
+      <c r="J16" s="43" t="s">
         <v>7544</v>
-      </c>
-      <c r="I16" s="45" t="s">
-        <v>7553</v>
-      </c>
-      <c r="J16" s="43" t="s">
-        <v>7546</v>
       </c>
     </row>
     <row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
@@ -25913,7 +25905,7 @@
         <v>7535</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>7562</v>
+        <v>7560</v>
       </c>
       <c r="C17" s="43" t="s">
         <v>7534</v>
@@ -25922,47 +25914,47 @@
         <v>1</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="42" t="s">
         <v>7523</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>7550</v>
+        <v>7548</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>7551</v>
+        <v>7549</v>
       </c>
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="43" t="s">
-        <v>7559</v>
+        <v>7557</v>
       </c>
       <c r="B18" s="43" t="s">
+        <v>7554</v>
+      </c>
+      <c r="C18" s="44" t="s">
         <v>7556</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>7558</v>
       </c>
       <c r="D18" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="42" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="H18" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>7543</v>
+      </c>
+      <c r="J18" s="43" t="s">
         <v>7544</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>7545</v>
-      </c>
-      <c r="J18" s="43" t="s">
-        <v>7546</v>
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
@@ -25971,29 +25963,29 @@
     </row>
     <row r="19" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="43" t="s">
-        <v>7554</v>
+        <v>7552</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>7557</v>
+        <v>7555</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>7539</v>
+        <v>7537</v>
       </c>
       <c r="D19" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>7543</v>
+      </c>
+      <c r="I19" s="43" t="s">
         <v>7544</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>7545</v>
-      </c>
-      <c r="I19" s="43" t="s">
-        <v>7546</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
@@ -26004,30 +25996,30 @@
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
       <c r="A20" s="43" t="s">
-        <v>7560</v>
+        <v>7558</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>7561</v>
+        <v>7559</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>7540</v>
+        <v>7538</v>
       </c>
       <c r="D20" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>7543</v>
+      </c>
+      <c r="J20" s="43" t="s">
         <v>7544</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>7545</v>
-      </c>
-      <c r="J20" s="43" t="s">
-        <v>7546</v>
       </c>
       <c r="L20"/>
       <c r="M20"/>
@@ -26036,32 +26028,32 @@
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
       <c r="A21" s="43" t="s">
-        <v>7542</v>
+        <v>7540</v>
       </c>
       <c r="B21" s="43" t="s">
         <v>7529</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>7541</v>
+        <v>7539</v>
       </c>
       <c r="D21" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>7538</v>
+        <v>7536</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="45" t="s">
+        <v>7541</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I21" s="24" t="s">
         <v>7543</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="J21" s="43" t="s">
         <v>7544</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>7545</v>
-      </c>
-      <c r="J21" s="43" t="s">
-        <v>7546</v>
       </c>
       <c r="L21"/>
       <c r="M21"/>
@@ -26070,28 +26062,28 @@
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
       <c r="A22" s="43" t="s">
-        <v>7563</v>
+        <v>7561</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>7569</v>
+        <v>7567</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>7564</v>
+        <v>7562</v>
       </c>
       <c r="D22" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>7537</v>
+        <v>7536</v>
       </c>
       <c r="G22" s="43" t="s">
+        <v>7564</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I22" s="43" t="s">
         <v>7566</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>7544</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>7568</v>
       </c>
       <c r="J22" s="43" t="s">
         <v>7524</v>

</xml_diff>

<commit_message>
pSB1 only del test
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="4065" windowWidth="12855" windowHeight="120"/>
+    <workbookView xWindow="-105" yWindow="4515" windowWidth="12855" windowHeight="120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7681" uniqueCount="7580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7673" uniqueCount="7576">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22800,21 +22800,6 @@
   </si>
   <si>
     <t xml:space="preserve">"cpmbat proven" at iGEM Tokyo tech and Waseda </t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>pSB3K3,pSB1C3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>pSB3K3</t>
-  </si>
-  <si>
-    <t>pSB6A1,pSB1C3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>pSB6A1</t>
     <phoneticPr fontId="20"/>
   </si>
 </sst>
@@ -23617,8 +23602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30:L31"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -24299,53 +24284,19 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="24" t="s">
-        <v>7577</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>49</v>
-      </c>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
       <c r="D30" s="22"/>
-      <c r="F30" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>7577</v>
-      </c>
-      <c r="J30" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L30" s="8">
-        <v>0</v>
-      </c>
+      <c r="G30" s="24"/>
+      <c r="L30" s="8"/>
       <c r="M30" s="40"/>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="24" t="s">
-        <v>7579</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>49</v>
-      </c>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
       <c r="D31" s="22"/>
-      <c r="F31" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>7579</v>
-      </c>
-      <c r="J31" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L31" s="8">
-        <v>0</v>
-      </c>
+      <c r="G31" s="24"/>
+      <c r="L31" s="8"/>
       <c r="M31" s="40"/>
     </row>
     <row r="32" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
@@ -25346,8 +25297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -25865,7 +25816,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="43" t="s">
@@ -25909,7 +25860,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>7546</v>
@@ -25939,7 +25890,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>7578</v>
+        <v>7535</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="24" t="s">
@@ -25969,7 +25920,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="42" t="s">
@@ -25996,7 +25947,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="42" t="s">
@@ -26030,7 +25981,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="24" t="s">
@@ -26063,7 +26014,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -26095,7 +26046,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>7576</v>
+        <v>7535</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="45" t="s">
@@ -26129,7 +26080,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>7578</v>
+        <v>7535</v>
       </c>
       <c r="G22" s="43" t="s">
         <v>7563</v>

</xml_diff>

<commit_message>
creating a basic part version of the cell-cell communication package for synthesis
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d\Documents\GitHub\Forked_iGEM-distribution\Cell Cell communication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Cell Cell communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D552BC-1F17-B246-91FC-5EC0B13AE27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="16665" windowHeight="6240" activeTab="1"/>
+    <workbookView xWindow="-34060" yWindow="1080" windowWidth="26640" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7750" uniqueCount="7608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7662" uniqueCount="7560">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22608,152 +22609,20 @@
   </si>
   <si>
     <t>1.0a2</t>
-  </si>
-  <si>
-    <t>B0030</t>
-  </si>
-  <si>
-    <t>B0015</t>
-    <phoneticPr fontId="20"/>
   </si>
   <si>
     <t>Daisuke Kiga and iGEM Waseda</t>
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>Plas-LuxI</t>
-  </si>
-  <si>
-    <t>Plux-LasI</t>
-  </si>
-  <si>
-    <t>K934012</t>
-  </si>
-  <si>
-    <t>K934022</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>S03119</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Ptet-LuxR</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>promoterless-LasI</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K081016</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>pSB1C3</t>
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>deltaP-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Plambda-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Plux/tet-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K934025</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K934024</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>B0034</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>E0040</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>B0015</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>K649000</t>
   </si>
   <si>
-    <t>C0061</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>R0062</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>C0078</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>B1006</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>R0040</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>C0062</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K081008</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Plux-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K395100</t>
-  </si>
-  <si>
-    <t>K193000</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K553003</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>constitutive production of LasR</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>J23100</t>
-  </si>
-  <si>
-    <t>J23100</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>C0179</t>
-  </si>
-  <si>
-    <t>C0179</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>B0034</t>
-  </si>
-  <si>
-    <t>B1006</t>
   </si>
   <si>
     <t>C0061</t>
@@ -22779,54 +22648,10 @@
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech, sender, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech, sender,pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech, sender negative control, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech,Reporter netgative control, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech,Reporter, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech,Reporter positive control, original at iGEM09_Tokyo_Tech, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Kiga lab 2021, original at iGEM11_UNITS_TRIESTE, pSB6A1</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM12_Tokyo_Tech, sender, pSB6A1</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM14_Tokyo_Tech, pSB3K3</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>K1529300</t>
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>J54103</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>K1529310</t>
     <phoneticPr fontId="20"/>
   </si>
@@ -22839,13 +22664,6 @@
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>K1949060</t>
-  </si>
-  <si>
-    <t>RRhl(MN) low crosstalk</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>C0070</t>
   </si>
   <si>
@@ -22857,30 +22675,6 @@
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>Prhl(RL)-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Plux-CmR-RhlI</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K1529797</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>K395160</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>C0070</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>RBS-CmR</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>C0071</t>
     <phoneticPr fontId="20"/>
   </si>
@@ -22893,50 +22687,60 @@
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>Prhl(LR)-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>variant of K1529300</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM16_Tokyo_Tech</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Prhl(NM)-GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>RhlR no LVA</t>
     <phoneticPr fontId="20"/>
   </si>
   <si>
-    <t>GFP</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Ptet RhlR</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> iGEM14_Tokyo_Tech, pSB6A1</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
-    <t>Ptet RhlR LVA</t>
-    <phoneticPr fontId="20"/>
-  </si>
-  <si>
     <t>C0171</t>
     <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>pSB1C5</t>
+  </si>
+  <si>
+    <t>D1005</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>L0 CDS 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>L0 CDS 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1001</t>
+  </si>
+  <si>
+    <t>L0 Promoter 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1002</t>
+  </si>
+  <si>
+    <t>L0 Promoter 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>C0061, C0062, C0078, C0179, C0071, C0171, C0070</t>
+  </si>
+  <si>
+    <t>Cell-Comm-CDS</t>
+  </si>
+  <si>
+    <t>Cell-Comm-Promoters</t>
+  </si>
+  <si>
+    <t>K649000, K934024, R0062, K1529300, K1529310, R0051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="25">
     <font>
       <sz val="12"/>
@@ -23293,7 +23097,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -23451,27 +23255,27 @@
     </dxf>
   </dxfs>
   <tableStyles count="5" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Basic Parts-style" pivot="0" count="3">
+    <tableStyle name="Basic Parts-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="firstRowStripe" dxfId="15"/>
       <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
       <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 2" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="firstRowStripe" dxfId="9"/>
       <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 3" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
       <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 4" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="firstRowStripe" dxfId="3"/>
       <tableStyleElement type="secondRowStripe" dxfId="2"/>
@@ -23489,44 +23293,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A14:M39" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M44" headerRowCount="0">
   <tableColumns count="13">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12" dataDxfId="1"/>
-    <tableColumn id="13" name="Column13" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_3" displayName="Table_3" ref="A13:O34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_3" displayName="Table_3" ref="A13:O34">
   <tableColumns count="15">
-    <tableColumn id="1" name="Part/Library Name"/>
-    <tableColumn id="2" name="Design Notes"/>
-    <tableColumn id="3" name="Part Description"/>
-    <tableColumn id="4" name="Final Product"/>
-    <tableColumn id="6" name="Backbone/locus"/>
-    <tableColumn id="7" name="Constraints"/>
-    <tableColumn id="8" name="Part 1"/>
-    <tableColumn id="9" name="Part 2"/>
-    <tableColumn id="10" name="Part 3"/>
-    <tableColumn id="11" name="Part 4"/>
-    <tableColumn id="12" name="Part 5"/>
-    <tableColumn id="13" name="Part 6"/>
-    <tableColumn id="14" name="Part 7"/>
-    <tableColumn id="15" name="Part 8"/>
-    <tableColumn id="16" name="Part 9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Part/Library Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Design Notes"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Part Description"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Final Product"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Backbone/locus"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Constraints"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Part 1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Part 2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Part 3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Part 4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Part 5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Part 6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Part 7"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Part 8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Part 9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23729,27 +23533,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" style="14" customWidth="1"/>
-    <col min="10" max="11" width="8.44140625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="34.44140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="14" customWidth="1"/>
+    <col min="10" max="11" width="8.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="14" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -23757,7 +23561,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>7567</v>
+        <v>7532</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="20" t="s">
@@ -23778,7 +23582,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>7525</v>
+        <v>7523</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -23824,9 +23628,9 @@
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
     </row>
-    <row r="5" spans="1:13" ht="45.95" customHeight="1">
+    <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="46" t="s">
-        <v>7568</v>
+        <v>7533</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -24080,17 +23884,17 @@
     </row>
     <row r="15" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>48</v>
+        <v>7546</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>49</v>
+        <v>4482</v>
       </c>
       <c r="D15" s="22"/>
       <c r="F15" s="19" t="s">
-        <v>8</v>
+        <v>7519</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>48</v>
+        <v>7546</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>9</v>
@@ -24106,16 +23910,19 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="24"/>
+      <c r="A16" s="43" t="s">
+        <v>7527</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="D16" s="22"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="42" t="s">
-        <v>58</v>
+      <c r="G16" s="43" t="s">
+        <v>7527</v>
       </c>
       <c r="J16" s="19" t="b">
         <v>0</v>
@@ -24128,16 +23935,19 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="42" t="s">
-        <v>7523</v>
-      </c>
-      <c r="B17" s="24"/>
+      <c r="A17" s="24" t="s">
+        <v>7528</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="D17" s="22"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="42" t="s">
-        <v>7523</v>
+      <c r="G17" s="24" t="s">
+        <v>7528</v>
       </c>
       <c r="J17" s="19" t="b">
         <v>0</v>
@@ -24150,16 +23960,18 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="24" t="s">
-        <v>7560</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="19" t="s">
+        <v>7529</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="24"/>
       <c r="F18" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="24" t="s">
-        <v>7560</v>
+      <c r="G18" s="19" t="s">
+        <v>7529</v>
       </c>
       <c r="J18" s="19" t="b">
         <v>0</v>
@@ -24173,14 +23985,16 @@
     </row>
     <row r="19" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>7561</v>
-      </c>
-      <c r="B19" s="24"/>
+        <v>7526</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="F19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>7561</v>
+        <v>7526</v>
       </c>
       <c r="J19" s="19" t="b">
         <v>0</v>
@@ -24194,17 +24008,21 @@
       <c r="M19" s="38"/>
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A20" s="43" t="s">
-        <v>7562</v>
-      </c>
-      <c r="B20" s="39"/>
+      <c r="A20" s="24" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>7542</v>
+      </c>
       <c r="D20" s="22"/>
-      <c r="E20" s="24"/>
       <c r="F20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="43" t="s">
-        <v>7562</v>
+      <c r="G20" s="24" t="s">
+        <v>7541</v>
       </c>
       <c r="J20" s="19" t="b">
         <v>0</v>
@@ -24218,16 +24036,20 @@
     </row>
     <row r="21" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>7563</v>
-      </c>
-      <c r="B21" s="39"/>
+        <v>7545</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>7544</v>
+      </c>
       <c r="D21" s="22"/>
-      <c r="E21" s="24"/>
       <c r="F21" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>7563</v>
+        <v>7545</v>
       </c>
       <c r="J21" s="19" t="b">
         <v>0</v>
@@ -24240,16 +24062,21 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="19" t="s">
-        <v>7564</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="24" t="s">
+        <v>7539</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>7540</v>
+      </c>
+      <c r="D22" s="22"/>
       <c r="F22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>7564</v>
+      <c r="G22" s="24" t="s">
+        <v>7538</v>
       </c>
       <c r="J22" s="19" t="b">
         <v>0</v>
@@ -24263,14 +24090,16 @@
     </row>
     <row r="23" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>7558</v>
-      </c>
-      <c r="B23" s="39"/>
+        <v>7525</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="F23" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>7558</v>
+        <v>7525</v>
       </c>
       <c r="J23" s="19" t="b">
         <v>0</v>
@@ -24284,15 +24113,17 @@
     </row>
     <row r="24" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="39"/>
+        <v>7530</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="D24" s="22"/>
       <c r="F24" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>57</v>
+        <v>7530</v>
       </c>
       <c r="J24" s="19" t="b">
         <v>0</v>
@@ -24306,15 +24137,17 @@
     </row>
     <row r="25" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>7556</v>
-      </c>
-      <c r="B25" s="39"/>
+        <v>7531</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="D25" s="22"/>
       <c r="F25" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>7556</v>
+        <v>7531</v>
       </c>
       <c r="J25" s="19" t="b">
         <v>0</v>
@@ -24327,15 +24160,21 @@
       </c>
     </row>
     <row r="26" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="24" t="s">
-        <v>7543</v>
-      </c>
-      <c r="B26" s="39"/>
+      <c r="A26" s="43" t="s">
+        <v>7534</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>7536</v>
+      </c>
+      <c r="D26" s="22"/>
       <c r="F26" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="24" t="s">
-        <v>7543</v>
+      <c r="G26" s="43" t="s">
+        <v>7534</v>
       </c>
       <c r="J26" s="19" t="b">
         <v>0</v>
@@ -24348,16 +24187,21 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="24" t="s">
-        <v>7565</v>
-      </c>
-      <c r="B27" s="39"/>
+      <c r="A27" s="43" t="s">
+        <v>7535</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>7537</v>
+      </c>
       <c r="D27" s="22"/>
       <c r="F27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="24" t="s">
-        <v>7565</v>
+      <c r="G27" s="43" t="s">
+        <v>7535</v>
       </c>
       <c r="J27" s="19" t="b">
         <v>0</v>
@@ -24371,15 +24215,17 @@
     </row>
     <row r="28" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="39"/>
+        <v>7543</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="D28" s="22"/>
       <c r="F28" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>69</v>
+        <v>7543</v>
       </c>
       <c r="J28" s="19" t="b">
         <v>0</v>
@@ -24392,17 +24238,11 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="24" t="s">
-        <v>7566</v>
-      </c>
-      <c r="B29" s="39"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="22"/>
-      <c r="F29" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>7566</v>
-      </c>
+      <c r="G29" s="43"/>
       <c r="J29" s="19" t="b">
         <v>0</v>
       </c>
@@ -24414,20 +24254,11 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="43" t="s">
-        <v>7579</v>
-      </c>
+      <c r="A30" s="43"/>
       <c r="B30" s="24"/>
-      <c r="C30" s="24" t="s">
-        <v>7582</v>
-      </c>
+      <c r="C30" s="24"/>
       <c r="D30" s="22"/>
-      <c r="F30" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="43" t="s">
-        <v>7579</v>
-      </c>
+      <c r="G30" s="43"/>
       <c r="J30" s="19" t="b">
         <v>0</v>
       </c>
@@ -24441,18 +24272,29 @@
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="43" t="s">
-        <v>7581</v>
-      </c>
-      <c r="B31" s="24"/>
+        <v>7547</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>1363</v>
+      </c>
       <c r="C31" s="24" t="s">
-        <v>7583</v>
+        <v>7548</v>
       </c>
       <c r="D31" s="22"/>
+      <c r="E31" s="19" t="s">
+        <v>7549</v>
+      </c>
       <c r="F31" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="43" t="s">
-        <v>7581</v>
+        <v>7547</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>7429</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="J31" s="19" t="b">
         <v>0</v>
@@ -24467,18 +24309,29 @@
     </row>
     <row r="32" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="43" t="s">
-        <v>7584</v>
-      </c>
-      <c r="B32" s="39"/>
+        <v>7550</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>1363</v>
+      </c>
       <c r="C32" s="24" t="s">
-        <v>7585</v>
+        <v>7548</v>
       </c>
       <c r="D32" s="22"/>
+      <c r="E32" s="19" t="s">
+        <v>7551</v>
+      </c>
       <c r="F32" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="43" t="s">
-        <v>7584</v>
+        <v>7550</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>7429</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="J32" s="19" t="b">
         <v>0</v>
@@ -24492,18 +24345,29 @@
     </row>
     <row r="33" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="43" t="s">
-        <v>7580</v>
-      </c>
-      <c r="B33" s="39"/>
+        <v>7552</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>1363</v>
+      </c>
       <c r="C33" s="24" t="s">
-        <v>7603</v>
+        <v>7548</v>
       </c>
       <c r="D33" s="22"/>
+      <c r="E33" s="19" t="s">
+        <v>7553</v>
+      </c>
       <c r="F33" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G33" s="43" t="s">
-        <v>7580</v>
+        <v>7552</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>7429</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="J33" s="19" t="b">
         <v>0</v>
@@ -24518,18 +24382,29 @@
     </row>
     <row r="34" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>7595</v>
-      </c>
-      <c r="B34" s="39"/>
+        <v>7554</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>1363</v>
+      </c>
       <c r="C34" s="24" t="s">
-        <v>7596</v>
+        <v>7548</v>
       </c>
       <c r="D34" s="22"/>
+      <c r="E34" s="19" t="s">
+        <v>7555</v>
+      </c>
       <c r="F34" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>7595</v>
+        <v>7554</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>7429</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="J34" s="19" t="b">
         <v>0</v>
@@ -24542,20 +24417,11 @@
       </c>
     </row>
     <row r="35" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="24" t="s">
-        <v>7607</v>
-      </c>
+      <c r="A35" s="24"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="24" t="s">
-        <v>7602</v>
-      </c>
+      <c r="C35" s="24"/>
       <c r="D35" s="22"/>
-      <c r="F35" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="24" t="s">
-        <v>7607</v>
-      </c>
+      <c r="G35" s="24"/>
       <c r="J35" s="19" t="b">
         <v>0</v>
       </c>
@@ -24567,20 +24433,11 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="24" t="s">
-        <v>7587</v>
-      </c>
+      <c r="A36" s="24"/>
       <c r="B36" s="24"/>
-      <c r="C36" s="24" t="s">
-        <v>7588</v>
-      </c>
+      <c r="C36" s="24"/>
       <c r="D36" s="22"/>
-      <c r="F36" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>7586</v>
-      </c>
+      <c r="G36" s="24"/>
       <c r="J36" s="19" t="b">
         <v>0</v>
       </c>
@@ -24592,20 +24449,11 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="43" t="s">
-        <v>7592</v>
-      </c>
+      <c r="A37" s="43"/>
       <c r="B37" s="24"/>
-      <c r="C37" s="24" t="s">
-        <v>7594</v>
-      </c>
+      <c r="C37" s="24"/>
       <c r="D37" s="22"/>
-      <c r="F37" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="43" t="s">
-        <v>7592</v>
-      </c>
+      <c r="G37" s="43"/>
       <c r="J37" s="19" t="b">
         <v>0</v>
       </c>
@@ -24617,17 +24465,10 @@
       </c>
     </row>
     <row r="38" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="24" t="s">
-        <v>7597</v>
-      </c>
+      <c r="A38" s="24"/>
       <c r="B38" s="24"/>
       <c r="D38" s="22"/>
-      <c r="F38" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="24" t="s">
-        <v>7597</v>
-      </c>
+      <c r="G38" s="24"/>
       <c r="J38" s="19" t="b">
         <v>0</v>
       </c>
@@ -24645,11 +24486,81 @@
       <c r="L39" s="37"/>
       <c r="M39" s="38"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="38"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="38"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="38"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="38"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="38"/>
+    </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
@@ -25579,33 +25490,57 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E234908-3A8B-6D4A-84E7-E517A0F2EB30}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15:B44</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DAE54E4-6F7B-C944-92A3-ADDD1FDBFD4E}">
+          <x14:formula1>
+            <xm:f>data_source!$B$2:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F15:F44</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77C4CDDD-7239-3E40-9255-9FE9657B9F2A}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J15:K44</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="14" customWidth="1"/>
     <col min="5" max="5" width="17" style="14" customWidth="1"/>
     <col min="6" max="6" width="15" style="14" customWidth="1"/>
-    <col min="7" max="12" width="20.88671875" style="14" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="14" customWidth="1"/>
-    <col min="14" max="15" width="8.6640625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" style="14" customWidth="1"/>
-    <col min="17" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="7" max="12" width="20.85546875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="14" customWidth="1"/>
+    <col min="14" max="15" width="8.7109375" style="14" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" style="14" customWidth="1"/>
+    <col min="17" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.95" customHeight="1">
+    <row r="1" spans="1:26" ht="16" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -25635,7 +25570,7 @@
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:26" ht="15.95" customHeight="1">
+    <row r="2" spans="1:26" ht="16" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -25665,7 +25600,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:26" ht="15.95" customHeight="1">
+    <row r="3" spans="1:26" ht="16" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
@@ -25703,7 +25638,7 @@
       <c r="Y3" s="19"/>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26" ht="15.95" customHeight="1">
+    <row r="4" spans="1:26" ht="16" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
@@ -25743,7 +25678,7 @@
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26" ht="15.95" customHeight="1">
+    <row r="5" spans="1:26" ht="16" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -25783,7 +25718,7 @@
       <c r="Y5" s="19"/>
       <c r="Z5" s="19"/>
     </row>
-    <row r="6" spans="1:26" ht="15.95" customHeight="1">
+    <row r="6" spans="1:26" ht="16" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>62</v>
       </c>
@@ -25819,7 +25754,7 @@
       <c r="Y6" s="19"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:26" ht="15.95" customHeight="1">
+    <row r="7" spans="1:26" ht="16" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -25831,7 +25766,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>7534</v>
+        <v>7524</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
@@ -25863,7 +25798,7 @@
       <c r="Y7" s="19"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26" ht="15.95" customHeight="1">
+    <row r="8" spans="1:26" ht="16" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>67</v>
       </c>
@@ -25929,7 +25864,7 @@
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
     </row>
-    <row r="10" spans="1:26" ht="15.95" customHeight="1">
+    <row r="10" spans="1:26" ht="16" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20" t="s">
@@ -25959,7 +25894,7 @@
       <c r="Y10" s="19"/>
       <c r="Z10" s="19"/>
     </row>
-    <row r="11" spans="1:26" ht="15.95" customHeight="1">
+    <row r="11" spans="1:26" ht="16" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>70</v>
       </c>
@@ -26093,29 +26028,25 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="43" t="s">
-        <v>7528</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>7569</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>7526</v>
-      </c>
+        <v>7557</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>7534</v>
+        <v>7546</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="43" t="s">
-        <v>7543</v>
+        <v>7547</v>
       </c>
       <c r="H14" s="42" t="s">
-        <v>7523</v>
+        <v>7556</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>7544</v>
+        <v>7550</v>
       </c>
       <c r="J14" s="36"/>
       <c r="K14" s="22"/>
@@ -26135,153 +26066,79 @@
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
     </row>
-    <row r="15" spans="1:26" s="19" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="1:26" s="19" customFormat="1" ht="16" customHeight="1">
       <c r="A15" s="43" t="s">
-        <v>7529</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>7570</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>7527</v>
-      </c>
+        <v>7558</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>7534</v>
+        <v>7546</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>7545</v>
+        <v>7552</v>
       </c>
       <c r="H15" s="42" t="s">
-        <v>7523</v>
+        <v>7559</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>7546</v>
-      </c>
-      <c r="J15" s="42" t="s">
-        <v>7547</v>
-      </c>
+        <v>7554</v>
+      </c>
+      <c r="J15" s="42"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="43" t="s">
-        <v>7530</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>7577</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>7531</v>
-      </c>
-      <c r="D16" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="24" t="s">
-        <v>7548</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I16" s="45" t="s">
-        <v>7549</v>
-      </c>
-      <c r="J16" s="43" t="s">
-        <v>7542</v>
-      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="43" t="s">
-        <v>7533</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>7571</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>7532</v>
-      </c>
-      <c r="D17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="42" t="s">
-        <v>7523</v>
-      </c>
-      <c r="H17" s="42" t="s">
-        <v>7546</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>7547</v>
-      </c>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="43" t="s">
-        <v>7552</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>7573</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>7551</v>
-      </c>
-      <c r="D18" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="42" t="s">
-        <v>7545</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>7541</v>
-      </c>
-      <c r="J18" s="43" t="s">
-        <v>7542</v>
-      </c>
+      <c r="G18" s="42"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="43"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="43" t="s">
-        <v>7550</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>7572</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>7535</v>
-      </c>
-      <c r="D19" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>7541</v>
-      </c>
-      <c r="I19" s="43" t="s">
-        <v>7542</v>
-      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="43"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -26290,264 +26147,116 @@
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="A20" s="43" t="s">
-        <v>7553</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>7575</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>7536</v>
-      </c>
-      <c r="D20" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="24" t="s">
-        <v>7597</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>7541</v>
-      </c>
-      <c r="J20" s="43" t="s">
-        <v>7542</v>
-      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="43"/>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="A21" s="43" t="s">
-        <v>7538</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>7574</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>7537</v>
-      </c>
-      <c r="D21" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="45" t="s">
-        <v>7539</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>7541</v>
-      </c>
-      <c r="J21" s="43" t="s">
-        <v>7542</v>
-      </c>
+      <c r="G21" s="45"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="43"/>
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="A22" s="43" t="s">
-        <v>7554</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>7576</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>7555</v>
-      </c>
-      <c r="D22" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>7534</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>7557</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>7559</v>
-      </c>
-      <c r="J22" s="43" t="s">
-        <v>7524</v>
-      </c>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="24"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="A23" s="43" t="s">
-        <v>7579</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>7578</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>7589</v>
-      </c>
-      <c r="D23" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>7534</v>
-      </c>
-      <c r="G23" s="43" t="s">
-        <v>7579</v>
-      </c>
-      <c r="H23" s="43" t="s">
-        <v>7580</v>
-      </c>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="24"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="43" t="s">
-        <v>7591</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>7578</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>7590</v>
-      </c>
-      <c r="D24" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>7534</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>7545</v>
-      </c>
-      <c r="H24" s="43" t="s">
-        <v>7592</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>7593</v>
-      </c>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="A25" s="43" t="s">
-        <v>7581</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>7578</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>7598</v>
-      </c>
-      <c r="D25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>7534</v>
-      </c>
-      <c r="G25" s="43" t="s">
-        <v>7581</v>
-      </c>
-      <c r="H25" s="43" t="s">
-        <v>7580</v>
-      </c>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="A26" s="43" t="s">
-        <v>7599</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>7600</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>7601</v>
-      </c>
-      <c r="D26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="43" t="s">
-        <v>7584</v>
-      </c>
-      <c r="H26" s="43" t="s">
-        <v>7580</v>
-      </c>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1">
-      <c r="A27" s="43" t="s">
-        <v>7606</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>7605</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>7604</v>
-      </c>
-      <c r="D27" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="24" t="s">
-        <v>7548</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>7595</v>
-      </c>
-      <c r="J27" s="43" t="s">
-        <v>7524</v>
-      </c>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1">
-      <c r="A28" s="43" t="s">
-        <v>7604</v>
-      </c>
+      <c r="A28" s="43"/>
       <c r="B28" s="43"/>
-      <c r="C28" s="43" t="s">
-        <v>7606</v>
-      </c>
-      <c r="D28" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>7534</v>
-      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="24" t="s">
-        <v>7548</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>7540</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>7607</v>
-      </c>
-      <c r="J28" s="43" t="s">
-        <v>7524</v>
-      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1">
       <c r="C29" s="44"/>
       <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
@@ -26611,11 +26320,23 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D99BB7B6-380B-FF49-B369-DE1CF1F1AB96}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D14:D34</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -26623,11 +26344,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="16" style="14" customWidth="1"/>
-    <col min="3" max="26" width="10.5546875" style="14" customWidth="1"/>
+    <col min="3" max="26" width="10.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
@@ -61510,13 +61231,13 @@
       <c r="C2535" s="29"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="C752" r:id="rId1"/>
-    <hyperlink ref="C2371" r:id="rId2"/>
-    <hyperlink ref="C2372" r:id="rId3"/>
-    <hyperlink ref="C2518" r:id="rId4"/>
+    <hyperlink ref="C752" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C2371" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C2372" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C2518" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -61524,7 +61245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -61537,14 +61258,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="14" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="14" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -62763,7 +62484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -62773,9 +62494,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -63869,8 +63590,8 @@
   </sheetData>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -63878,7 +63599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -63886,14 +63607,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="14" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="14" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -67113,33 +66834,33 @@
   </sheetData>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
-    <hyperlink ref="C4" r:id="rId7"/>
-    <hyperlink ref="D4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9"/>
-    <hyperlink ref="C5" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="F5" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="D6" r:id="rId14"/>
-    <hyperlink ref="F6" r:id="rId15"/>
-    <hyperlink ref="C7" r:id="rId16"/>
-    <hyperlink ref="D7" r:id="rId17"/>
-    <hyperlink ref="F7" r:id="rId18"/>
-    <hyperlink ref="D8" r:id="rId19"/>
-    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="F5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="C6" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="D6" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="C7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="D7" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="F7" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -67149,10 +66870,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="14" customWidth="1"/>
-    <col min="2" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="14" customWidth="1"/>
+    <col min="2" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
added in missing promoter that was part of a composite
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Cell Cell communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D552BC-1F17-B246-91FC-5EC0B13AE27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAC550-0A2B-5C42-BA93-9A69EDA615E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34060" yWindow="1080" windowWidth="26640" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7662" uniqueCount="7560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7667" uniqueCount="7563">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22734,7 +22734,16 @@
     <t>Cell-Comm-Promoters</t>
   </si>
   <si>
-    <t>K649000, K934024, R0062, K1529300, K1529310, R0051</t>
+    <t>TCCTGTGAAATCTGGCAGTTACCGTTAGCTTTCGAATTGGCTAtAAAGTGTTC</t>
+  </si>
+  <si>
+    <t>Prhl(NM) from BBa_K1949060</t>
+  </si>
+  <si>
+    <t>Prhl_NM</t>
+  </si>
+  <si>
+    <t>K649000, K934024, R0062, K1529300, K1529310, R0051, Prhl_NM</t>
   </si>
 </sst>
 </file>
@@ -23039,7 +23048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23077,7 +23086,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -23536,8 +23544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23629,14 +23637,14 @@
       <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="45" t="s">
         <v>7533</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -23906,14 +23914,15 @@
         <v>1</v>
       </c>
       <c r="L15" s="8">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>7527</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D16" s="22"/>
@@ -23921,7 +23930,7 @@
       <c r="F16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="42" t="s">
         <v>7527</v>
       </c>
       <c r="J16" s="19" t="b">
@@ -23931,6 +23940,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="8">
+        <f t="shared" ref="L16:L44" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M16,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
     </row>
@@ -23938,7 +23948,7 @@
       <c r="A17" s="24" t="s">
         <v>7528</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D17" s="22"/>
@@ -23956,6 +23966,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23963,7 +23974,7 @@
       <c r="A18" s="19" t="s">
         <v>7529</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="38" t="s">
         <v>90</v>
       </c>
       <c r="C18" s="24"/>
@@ -23980,6 +23991,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -23987,7 +23999,7 @@
       <c r="A19" s="24" t="s">
         <v>7526</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="38" t="s">
         <v>90</v>
       </c>
       <c r="F19" s="19" t="s">
@@ -24003,15 +24015,16 @@
         <v>0</v>
       </c>
       <c r="L19" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M19" s="38"/>
+      <c r="M19" s="37"/>
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="24" t="s">
         <v>7541</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="38" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="24" t="s">
@@ -24031,6 +24044,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24058,6 +24072,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24085,6 +24100,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24092,7 +24108,7 @@
       <c r="A23" s="24" t="s">
         <v>7525</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="38" t="s">
         <v>47</v>
       </c>
       <c r="F23" s="19" t="s">
@@ -24108,6 +24124,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24115,7 +24132,7 @@
       <c r="A24" s="24" t="s">
         <v>7530</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="38" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="22"/>
@@ -24132,6 +24149,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24139,7 +24157,7 @@
       <c r="A25" s="24" t="s">
         <v>7531</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="22"/>
@@ -24156,11 +24174,12 @@
         <v>0</v>
       </c>
       <c r="L25" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>7534</v>
       </c>
       <c r="B26" s="24" t="s">
@@ -24173,7 +24192,7 @@
       <c r="F26" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="43" t="s">
+      <c r="G26" s="42" t="s">
         <v>7534</v>
       </c>
       <c r="J26" s="19" t="b">
@@ -24183,11 +24202,12 @@
         <v>0</v>
       </c>
       <c r="L26" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="42" t="s">
         <v>7535</v>
       </c>
       <c r="B27" s="24" t="s">
@@ -24200,7 +24220,7 @@
       <c r="F27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="42" t="s">
         <v>7535</v>
       </c>
       <c r="J27" s="19" t="b">
@@ -24210,6 +24230,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24234,15 +24255,24 @@
         <v>0</v>
       </c>
       <c r="L28" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="A29" s="42" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>7560</v>
+      </c>
       <c r="D29" s="22"/>
-      <c r="G29" s="43"/>
+      <c r="G29" s="42" t="s">
+        <v>7561</v>
+      </c>
       <c r="J29" s="19" t="b">
         <v>0</v>
       </c>
@@ -24250,15 +24280,19 @@
         <v>0</v>
       </c>
       <c r="L29" s="8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="M29" s="19" t="s">
+        <v>7559</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="43"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
       <c r="D30" s="22"/>
-      <c r="G30" s="43"/>
+      <c r="G30" s="42"/>
       <c r="J30" s="19" t="b">
         <v>0</v>
       </c>
@@ -24266,12 +24300,13 @@
         <v>0</v>
       </c>
       <c r="L30" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="40"/>
+      <c r="M30" s="39"/>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>7547</v>
       </c>
       <c r="B31" s="24" t="s">
@@ -24287,7 +24322,7 @@
       <c r="F31" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="43" t="s">
+      <c r="G31" s="42" t="s">
         <v>7547</v>
       </c>
       <c r="H31" s="19" t="s">
@@ -24303,15 +24338,16 @@
         <v>0</v>
       </c>
       <c r="L31" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M31" s="40"/>
+      <c r="M31" s="39"/>
     </row>
     <row r="32" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="42" t="s">
         <v>7550</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="38" t="s">
         <v>1363</v>
       </c>
       <c r="C32" s="24" t="s">
@@ -24324,7 +24360,7 @@
       <c r="F32" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="43" t="s">
+      <c r="G32" s="42" t="s">
         <v>7550</v>
       </c>
       <c r="H32" s="19" t="s">
@@ -24340,14 +24376,15 @@
         <v>0</v>
       </c>
       <c r="L32" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="42" t="s">
         <v>7552</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="38" t="s">
         <v>1363</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -24360,7 +24397,7 @@
       <c r="F33" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="43" t="s">
+      <c r="G33" s="42" t="s">
         <v>7552</v>
       </c>
       <c r="H33" s="19" t="s">
@@ -24376,15 +24413,16 @@
         <v>0</v>
       </c>
       <c r="L33" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M33" s="41"/>
+      <c r="M33" s="40"/>
     </row>
     <row r="34" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="24" t="s">
         <v>7554</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="38" t="s">
         <v>1363</v>
       </c>
       <c r="C34" s="24" t="s">
@@ -24413,6 +24451,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24429,6 +24468,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24445,15 +24485,16 @@
         <v>0</v>
       </c>
       <c r="L36" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="43"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
       <c r="D37" s="22"/>
-      <c r="G37" s="43"/>
+      <c r="G37" s="42"/>
       <c r="J37" s="19" t="b">
         <v>0</v>
       </c>
@@ -24461,6 +24502,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24476,6 +24518,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -24483,8 +24526,11 @@
       <c r="A39" s="24"/>
       <c r="B39" s="24"/>
       <c r="G39" s="24"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="38"/>
+      <c r="L39" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="37"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="24"/>
@@ -24498,8 +24544,11 @@
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="38"/>
+      <c r="L40" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="37"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
       <c r="A41" s="24"/>
@@ -24513,8 +24562,11 @@
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="38"/>
+      <c r="L41" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="37"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
       <c r="A42" s="24"/>
@@ -24528,8 +24580,11 @@
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="38"/>
+      <c r="L42" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="37"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" s="24"/>
@@ -24543,8 +24598,11 @@
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="38"/>
+      <c r="L43" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="37"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
       <c r="A44" s="24"/>
@@ -24558,8 +24616,11 @@
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="38"/>
+      <c r="L44" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="37"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
@@ -25522,7 +25583,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26027,11 +26088,11 @@
       <c r="Z13" s="19"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>7557</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="19" t="b">
         <v>1</v>
       </c>
@@ -26039,10 +26100,10 @@
         <v>7546</v>
       </c>
       <c r="F14" s="19"/>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="42" t="s">
         <v>7547</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="41" t="s">
         <v>7556</v>
       </c>
       <c r="I14" s="36" t="s">
@@ -26067,78 +26128,78 @@
       <c r="Z14" s="19"/>
     </row>
     <row r="15" spans="1:26" s="19" customFormat="1" ht="16" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>7558</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>7546</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>7552</v>
       </c>
-      <c r="H15" s="42" t="s">
-        <v>7559</v>
-      </c>
-      <c r="I15" s="42" t="s">
+      <c r="H15" s="41" t="s">
+        <v>7562</v>
+      </c>
+      <c r="I15" s="41" t="s">
         <v>7554</v>
       </c>
-      <c r="J15" s="42"/>
+      <c r="J15" s="41"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="19"/>
       <c r="E16" s="24"/>
       <c r="F16" s="19"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="43"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="19"/>
       <c r="E17" s="24"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="19"/>
       <c r="E18" s="24"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="42"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="43"/>
+      <c r="J18" s="42"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="19"/>
       <c r="E19" s="24"/>
       <c r="F19" s="19"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
-      <c r="I19" s="43"/>
+      <c r="I19" s="42"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -26147,114 +26208,114 @@
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="19"/>
       <c r="E20" s="24"/>
       <c r="F20" s="19"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
-      <c r="J20" s="43"/>
+      <c r="J20" s="42"/>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="19"/>
       <c r="E21" s="24"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="45"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="43"/>
+      <c r="J21" s="42"/>
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="19"/>
       <c r="E22" s="24"/>
-      <c r="G22" s="43"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="19"/>
       <c r="E23" s="24"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="19"/>
       <c r="E24" s="24"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="43"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
       <c r="I24" s="24"/>
-      <c r="J24" s="45"/>
+      <c r="J24" s="44"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="19"/>
       <c r="E25" s="24"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="19"/>
       <c r="E26" s="24"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
       <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="19"/>
       <c r="E27" s="24"/>
       <c r="F27" s="19"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
-      <c r="J27" s="43"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="19"/>
       <c r="E28" s="24"/>
       <c r="F28" s="19"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="43"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1">
-      <c r="C29" s="44"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="19"/>
       <c r="E29" s="24"/>
       <c r="F29" s="19"/>
@@ -26263,9 +26324,9 @@
       <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="19"/>
       <c r="E30" s="24"/>
       <c r="F30" s="19"/>
@@ -26274,7 +26335,7 @@
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1">
-      <c r="C31" s="44"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -26283,9 +26344,9 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="19"/>
       <c r="E32" s="24"/>
       <c r="F32" s="19"/>
@@ -26294,7 +26355,7 @@
       <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1">
-      <c r="C33" s="44"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -26303,9 +26364,9 @@
       <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="19"/>
       <c r="E34" s="24"/>
       <c r="F34" s="19"/>

</xml_diff>

<commit_message>
small fixes, adding padding to cell-cell comm and plant parts, setting metal to false for build
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Cell Cell communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAC550-0A2B-5C42-BA93-9A69EDA615E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4DC4D8-278E-E641-A6DE-BFA36AFB8529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34060" yWindow="1080" windowWidth="26640" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34060" yWindow="1080" windowWidth="26640" windowHeight="14040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7667" uniqueCount="7563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7681" uniqueCount="7566">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22744,6 +22744,15 @@
   </si>
   <si>
     <t>K649000, K934024, R0062, K1529300, K1529310, R0051, Prhl_NM</t>
+  </si>
+  <si>
+    <t>D2001</t>
+  </si>
+  <si>
+    <t>Extra nonsense bases for synthesis</t>
+  </si>
+  <si>
+    <t>D2002</t>
   </si>
 </sst>
 </file>
@@ -23544,8 +23553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24456,11 +24465,25 @@
       </c>
     </row>
     <row r="35" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
+      <c r="A35" s="24" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>7564</v>
+      </c>
       <c r="D35" s="22"/>
-      <c r="G35" s="24"/>
+      <c r="F35" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>7563</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>7429</v>
+      </c>
       <c r="J35" s="19" t="b">
         <v>0</v>
       </c>
@@ -24473,11 +24496,25 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="24" t="s">
+        <v>7565</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>7564</v>
+      </c>
       <c r="D36" s="22"/>
-      <c r="G36" s="24"/>
+      <c r="F36" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>7565</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>7429</v>
+      </c>
       <c r="J36" s="19" t="b">
         <v>0</v>
       </c>
@@ -25582,8 +25619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26139,17 +26176,21 @@
       <c r="E15" s="24" t="s">
         <v>7546</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="19" t="s">
+        <v>7563</v>
+      </c>
+      <c r="H15" s="41" t="s">
         <v>7552</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="I15" s="41" t="s">
         <v>7562</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="J15" s="41" t="s">
         <v>7554</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="22"/>
+      <c r="K15" s="22" t="s">
+        <v>7565</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="42"/>

</xml_diff>

<commit_message>
Just missing the Interlab Constructs. Note for issue: Promoters_pBetI exists in TetR Orthologs & in Small Mol Inducers...but the sequence is different. Will open an issue for better checking.
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Cell Cell communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4DC4D8-278E-E641-A6DE-BFA36AFB8529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D82CD-C413-F846-ACAB-662A0FA548CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34060" yWindow="1080" windowWidth="26640" windowHeight="14040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7681" uniqueCount="7566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="7571">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22743,9 +22743,6 @@
     <t>Prhl_NM</t>
   </si>
   <si>
-    <t>K649000, K934024, R0062, K1529300, K1529310, R0051, Prhl_NM</t>
-  </si>
-  <si>
     <t>D2001</t>
   </si>
   <si>
@@ -22753,13 +22750,31 @@
   </si>
   <si>
     <t>D2002</t>
+  </si>
+  <si>
+    <t>Unable to build Cell-Comm-Promoters</t>
+  </si>
+  <si>
+    <t>K649000, K934024, R0062, K1529300, K1529310, Prhl_NM</t>
+  </si>
+  <si>
+    <t>R0051</t>
+  </si>
+  <si>
+    <t>Cell-Comm-Promoters in pSB1C3</t>
+  </si>
+  <si>
+    <t>Constructs belonged to original build plan, but unable to synthesize as clonal product by TWIST</t>
+  </si>
+  <si>
+    <t>Synthesized as linear fragments and cloned into pSB1C3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22921,6 +22936,12 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -23057,7 +23078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23112,6 +23133,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23553,8 +23575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:H36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24297,16 +24319,28 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="42"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>4482</v>
+      </c>
       <c r="C30" s="24"/>
       <c r="D30" s="22"/>
-      <c r="G30" s="42"/>
+      <c r="F30" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="J30" s="19" t="b">
         <v>0</v>
       </c>
       <c r="K30" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="8">
         <f t="shared" si="0"/>
@@ -24466,20 +24500,20 @@
     </row>
     <row r="35" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="24" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>1363</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="D35" s="22"/>
       <c r="F35" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>7429</v>
@@ -24497,20 +24531,20 @@
     </row>
     <row r="36" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="24" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>1363</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="D36" s="22"/>
       <c r="F36" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>7429</v>
@@ -25619,8 +25653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26177,43 +26211,82 @@
         <v>7546</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="H15" s="41" t="s">
         <v>7552</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>7562</v>
+        <v>7566</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>7554</v>
       </c>
       <c r="K15" s="22" t="s">
+        <v>7564</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="42" t="s">
         <v>7565</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="B16" s="48" t="s">
+        <v>7569</v>
+      </c>
       <c r="C16" s="42"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="24"/>
+      <c r="D16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>7546</v>
+      </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="42"/>
+      <c r="G16" s="19" t="s">
+        <v>7562</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>7552</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>7567</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>7554</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>7564</v>
+      </c>
     </row>
     <row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="42" t="s">
+        <v>7568</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>7570</v>
+      </c>
       <c r="C17" s="42"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="24"/>
+      <c r="D17" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="G17" s="19" t="s">
+        <v>7562</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>7552</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>7567</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>7554</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>7564</v>
+      </c>
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="42"/>

</xml_diff>

<commit_message>
updated the builds for packages based on the synthesis tracker. - "did not build" was used for parts planned for build, but removed because they were not Type IIS compatible - "unable to build" was used for parts planned for build, but could not be synthesized by TWIST (whether due to TWIST's pre-synthesis validation, or in actual product delivery)
</commit_message>
<xml_diff>
--- a/Cell Cell communication/cell cell communication.xlsx
+++ b/Cell Cell communication/cell cell communication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Cell Cell communication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D82CD-C413-F846-ACAB-662A0FA548CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA219F-2569-A24C-BBC9-2BAFF22AB386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21420" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="7571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="7577">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22725,9 +22725,6 @@
     <t>L0 Promoter 3' Flanking Region</t>
   </si>
   <si>
-    <t>C0061, C0062, C0078, C0179, C0071, C0171, C0070</t>
-  </si>
-  <si>
     <t>Cell-Comm-CDS</t>
   </si>
   <si>
@@ -22755,9 +22752,6 @@
     <t>Unable to build Cell-Comm-Promoters</t>
   </si>
   <si>
-    <t>K649000, K934024, R0062, K1529300, K1529310, Prhl_NM</t>
-  </si>
-  <si>
     <t>R0051</t>
   </si>
   <si>
@@ -22768,13 +22762,37 @@
   </si>
   <si>
     <t>Synthesized as linear fragments and cloned into pSB1C3</t>
+  </si>
+  <si>
+    <t>C0062, C0179, C0070</t>
+  </si>
+  <si>
+    <t>C0061, C0071, C0078, C0171</t>
+  </si>
+  <si>
+    <t>K649000, K1529300, Prhl_NM</t>
+  </si>
+  <si>
+    <t>Did not build Cell-Comm-Promoters</t>
+  </si>
+  <si>
+    <t>Did not build Cell-Comm-CDS</t>
+  </si>
+  <si>
+    <t>K1529310, R0062</t>
+  </si>
+  <si>
+    <t>R0051, K1529310, K934024, K934024, R0062</t>
+  </si>
+  <si>
+    <t>Constructs belonged to original build plan, but did not synthesize due to Type IIS incompatible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22942,6 +22960,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -23078,7 +23102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23128,12 +23152,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23575,7 +23600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -23668,14 +23693,14 @@
       <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="46" t="s">
         <v>7533</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -24292,17 +24317,17 @@
     </row>
     <row r="29" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="42" t="s">
-        <v>7561</v>
+        <v>7560</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>7560</v>
+        <v>7559</v>
       </c>
       <c r="D29" s="22"/>
       <c r="G29" s="42" t="s">
-        <v>7561</v>
+        <v>7560</v>
       </c>
       <c r="J29" s="19" t="b">
         <v>0</v>
@@ -24315,7 +24340,7 @@
         <v>53</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>7559</v>
+        <v>7558</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
@@ -24500,20 +24525,20 @@
     </row>
     <row r="35" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="24" t="s">
-        <v>7562</v>
+        <v>7561</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>1363</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="D35" s="22"/>
       <c r="F35" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>7562</v>
+        <v>7561</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>7429</v>
@@ -24531,20 +24556,20 @@
     </row>
     <row r="36" spans="1:13" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="24" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>1363</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="D36" s="22"/>
       <c r="F36" s="19" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>7429</v>
@@ -25653,8 +25678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26160,7 +26185,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="42" t="s">
-        <v>7557</v>
+        <v>7556</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="43"/>
@@ -26174,8 +26199,8 @@
       <c r="G14" s="42" t="s">
         <v>7547</v>
       </c>
-      <c r="H14" s="41" t="s">
-        <v>7556</v>
+      <c r="H14" s="45" t="s">
+        <v>7569</v>
       </c>
       <c r="I14" s="36" t="s">
         <v>7550</v>
@@ -26200,7 +26225,7 @@
     </row>
     <row r="15" spans="1:26" s="19" customFormat="1" ht="16" customHeight="1">
       <c r="A15" s="42" t="s">
-        <v>7558</v>
+        <v>7557</v>
       </c>
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
@@ -26211,27 +26236,27 @@
         <v>7546</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>7562</v>
-      </c>
-      <c r="H15" s="41" t="s">
+        <v>7561</v>
+      </c>
+      <c r="H15" s="45" t="s">
         <v>7552</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>7566</v>
+        <v>7571</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>7554</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="42" t="s">
-        <v>7565</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>7569</v>
+        <v>7564</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>7567</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="19" t="b">
@@ -26242,27 +26267,27 @@
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19" t="s">
-        <v>7562</v>
-      </c>
-      <c r="H16" s="41" t="s">
+        <v>7561</v>
+      </c>
+      <c r="H16" s="45" t="s">
         <v>7552</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>7567</v>
+        <v>7575</v>
       </c>
       <c r="J16" s="41" t="s">
         <v>7554</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
     </row>
     <row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="42" t="s">
+        <v>7566</v>
+      </c>
+      <c r="B17" s="45" t="s">
         <v>7568</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>7570</v>
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="19" t="b">
@@ -26273,31 +26298,45 @@
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19" t="s">
-        <v>7562</v>
-      </c>
-      <c r="H17" s="41" t="s">
+        <v>7561</v>
+      </c>
+      <c r="H17" s="45" t="s">
         <v>7552</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>7567</v>
+        <v>7565</v>
       </c>
       <c r="J17" s="41" t="s">
         <v>7554</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="42" t="s">
+        <v>7573</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>7576</v>
+      </c>
       <c r="C18" s="43"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>7546</v>
+      </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="G18" s="41" t="s">
+        <v>7547</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>7570</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>7550</v>
+      </c>
       <c r="J18" s="42"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
@@ -26305,17 +26344,35 @@
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="24"/>
+      <c r="A19" s="42" t="s">
+        <v>7572</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>7576</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>7546</v>
+      </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="G19" s="19" t="s">
+        <v>7561</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>7552</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>7574</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>7554</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>7563</v>
+      </c>
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>

</xml_diff>